<commit_message>
Final comments and code cleanup
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\kavya\Process-Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2764BB98-5D39-47B9-951A-E8A4209A5FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AA52F4-2276-4E54-BA49-72B3C2908E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{07BE8C77-AB8B-49FA-92E5-355528E98633}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -86,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2829,6 +2842,7 @@
         <c:axId val="1203667775"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5598,13 +5612,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E837100-ECF8-4564-BFCC-D66B19F137E9}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="51" workbookViewId="0">
-      <selection activeCell="AA39" sqref="AA39"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5639,7 +5653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -5677,7 +5691,7 @@
         <v>41042.35353</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -5715,7 +5729,7 @@
         <v>11400.3308</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -5753,7 +5767,7 @@
         <v>10064.47587</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5776,7 +5790,7 @@
         <v>94.68</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5811,7 +5825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5846,7 +5860,7 @@
         <v>39979.266159999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -5881,7 +5895,7 @@
         <v>11197.07416</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -5916,7 +5930,7 @@
         <v>9847.820205</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -5939,7 +5953,7 @@
         <v>97.43</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5974,7 +5988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -6009,7 +6023,7 @@
         <v>2700.0799889999998</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -6044,7 +6058,7 @@
         <v>1590.2993959999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -6079,7 +6093,7 @@
         <v>1.3939312909999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -6102,7 +6116,7 @@
         <v>34.15</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -6137,7 +6151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -6172,7 +6186,7 @@
         <v>2688.223027</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -6207,7 +6221,7 @@
         <v>2005.444757</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -6242,7 +6256,7 @@
         <v>1.4698401270000001</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -6265,7 +6279,7 @@
         <v>37.72</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -6288,7 +6302,7 @@
         <v>34.75</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -6311,7 +6325,7 @@
         <v>94.57</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -6334,7 +6348,7 @@
         <v>94.46</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -6357,7 +6371,7 @@
         <v>96.59</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -6380,7 +6394,7 @@
         <v>97.34</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -6403,7 +6417,7 @@
         <v>94.62</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -6426,7 +6440,7 @@
         <v>97.38</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -6449,7 +6463,7 @@
         <v>97.25</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -6472,7 +6486,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -6495,7 +6509,7 @@
         <v>95.12</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>

</xml_diff>